<commit_message>
microclimUS has wind speed and snow depth
</commit_message>
<xml_diff>
--- a/Data/DatasetTable.xlsx
+++ b/Data/DatasetTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yutaro\Documents\RShiny_Microclim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ameyer/RShiny_Microclim/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15DD0CD-DCB1-406D-A04A-0CB4F47D7970}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A142DF-5C44-554C-9E99-A668BA704B78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatasetTable" sheetId="1" r:id="rId1"/>
@@ -989,16 +989,16 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L8" t="s">
         <v>18</v>
@@ -1365,10 +1365,10 @@
         <v>17</v>
       </c>
       <c r="O8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
downscale USCRN. downsize microclimUS data files
</commit_message>
<xml_diff>
--- a/Data/DatasetTable.xlsx
+++ b/Data/DatasetTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ameyer/RShiny_Microclim/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264E2AC9-6FFB-7C4D-81E9-5CCA64112BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EA2CF5-9E13-2F47-A379-411F0FF0BF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>